<commit_message>
troche wyczyszczony kod i plik excel
</commit_message>
<xml_diff>
--- a/DATA/3.Wypadki_wg_przyczyn_WOJ.xlsx
+++ b/DATA/3.Wypadki_wg_przyczyn_WOJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natal\OneDrive\Dokumenty\AnalizaDanych\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A25F3BA-5CF8-4472-8B3F-DD3FCE704B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D957FDE-6FE9-4969-8F5E-645FDA267B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-330" yWindow="720" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="4785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -34,27 +34,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="29">
   <si>
     <t>Rok</t>
-  </si>
-  <si>
-    <t>Wina kierujących pojazdami ogółem</t>
-  </si>
-  <si>
-    <t>Wina kierujących pojazdami - niedostosowanie prędkości do warunków ruchu</t>
-  </si>
-  <si>
-    <t>Wina kierujących pojazdami - nieprzestrzeganie pierwszeństwa przejazdu</t>
-  </si>
-  <si>
-    <t>Wina kierujących pojazdami - nieprawidłowe wyprzedzanie</t>
-  </si>
-  <si>
-    <t>Wina kierujących pojazdami - nieprawidłowe zachowanie wobec pieszych</t>
-  </si>
-  <si>
-    <t>Wina kierujących pojazdami - niezachowanie bezpiecznej odległości między pojazdami</t>
-  </si>
-  <si>
-    <t>Wina kierujących pojazdami - pozostałe</t>
   </si>
   <si>
     <t>Wina pieszych - ogółem</t>
@@ -118,6 +97,27 @@
   </si>
   <si>
     <t>Wina pieszych - pozostałe</t>
+  </si>
+  <si>
+    <t>Wina kierowców ogółem</t>
+  </si>
+  <si>
+    <t>Wina kierowców - niedostosowanie prędkości</t>
+  </si>
+  <si>
+    <t>Wina kierowców - nieprzestrzeganie pierwszeństwa</t>
+  </si>
+  <si>
+    <t>Wina kierowców - nieprawidłowe wyprzedzanie</t>
+  </si>
+  <si>
+    <t>Wina kierowców - nieprawidłowe zachowanie wobec pieszych</t>
+  </si>
+  <si>
+    <t>Wina kierowców - niezachowanie bezpiecznej odległości</t>
+  </si>
+  <si>
+    <t>Wina kierowców - pozostałe</t>
   </si>
 </sst>
 </file>
@@ -261,13 +261,13 @@
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{F931E6CA-7BC0-4204-A56E-D5101E61B320}" name="Jednostka"/>
     <tableColumn id="2" xr3:uid="{566CFD72-3775-45F9-A648-40AA15C00AB9}" name="Rok"/>
-    <tableColumn id="3" xr3:uid="{946830C7-8424-4A8D-9047-C1E9087530BA}" name="Wina kierujących pojazdami ogółem" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{F92E356F-7E44-4759-8A45-8E7A636BC6E7}" name="Wina kierujących pojazdami - niedostosowanie prędkości do warunków ruchu" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{16CDF51B-E920-4545-A734-9965171033EE}" name="Wina kierujących pojazdami - nieprzestrzeganie pierwszeństwa przejazdu" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{83220930-617D-426C-8C2C-CE7BD6B4A5BF}" name="Wina kierujących pojazdami - nieprawidłowe wyprzedzanie" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{992AB53A-D61E-49C1-A321-6C2516C6D642}" name="Wina kierujących pojazdami - nieprawidłowe zachowanie wobec pieszych" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{F5AEE3EA-1C5A-4EA1-8FD6-1BC3F437A817}" name="Wina kierujących pojazdami - niezachowanie bezpiecznej odległości między pojazdami" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{F37FB52A-8DBD-44D1-AAE9-F89CB71549F0}" name="Wina kierujących pojazdami - pozostałe" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{946830C7-8424-4A8D-9047-C1E9087530BA}" name="Wina kierowców ogółem" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{F92E356F-7E44-4759-8A45-8E7A636BC6E7}" name="Wina kierowców - niedostosowanie prędkości" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{16CDF51B-E920-4545-A734-9965171033EE}" name="Wina kierowców - nieprzestrzeganie pierwszeństwa" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{83220930-617D-426C-8C2C-CE7BD6B4A5BF}" name="Wina kierowców - nieprawidłowe wyprzedzanie" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{992AB53A-D61E-49C1-A321-6C2516C6D642}" name="Wina kierowców - nieprawidłowe zachowanie wobec pieszych" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{F5AEE3EA-1C5A-4EA1-8FD6-1BC3F437A817}" name="Wina kierowców - niezachowanie bezpiecznej odległości" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{F37FB52A-8DBD-44D1-AAE9-F89CB71549F0}" name="Wina kierowców - pozostałe" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{1B680733-C603-4C47-BAFF-6648A6290240}" name="Wina pieszych - ogółem" dataDxfId="2"/>
     <tableColumn id="11" xr3:uid="{65DD9ADC-3B48-4707-AA31-17230B7374D5}" name="Wina pieszych - nieostrożne wejście na jezdnię" dataDxfId="1"/>
     <tableColumn id="12" xr3:uid="{25F2F24B-DEBB-4CEA-B493-DD377E9CE8A4}" name="Wina pieszych - pozostałe" dataDxfId="0"/>
@@ -576,66 +576,66 @@
   <dimension ref="A1:L120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" customWidth="1"/>
-    <col min="4" max="4" width="68" customWidth="1"/>
-    <col min="5" max="5" width="64.42578125" customWidth="1"/>
-    <col min="6" max="6" width="54.7109375" customWidth="1"/>
-    <col min="7" max="7" width="67.42578125" customWidth="1"/>
-    <col min="8" max="8" width="76.140625" customWidth="1"/>
-    <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="46.28515625" customWidth="1"/>
+    <col min="11" max="11" width="46" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2014</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>2014</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>2014</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>2014</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>2014</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>2014</v>
@@ -863,7 +863,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>2014</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>2014</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>2014</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>2014</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>2014</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>2014</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>2014</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>2014</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>2014</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>2014</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>2014</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B19">
         <v>2015</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <v>2015</v>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B21">
         <v>2015</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B22">
         <v>2015</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B23">
         <v>2015</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B24">
         <v>2015</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <v>2015</v>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>2015</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>2015</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B28">
         <v>2015</v>
@@ -1661,7 +1661,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B29">
         <v>2015</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B30">
         <v>2015</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B31">
         <v>2015</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B32">
         <v>2015</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B33">
         <v>2015</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B34">
         <v>2015</v>
@@ -1889,7 +1889,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B35">
         <v>2015</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B36">
         <v>2016</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B37">
         <v>2016</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B38">
         <v>2016</v>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B39">
         <v>2016</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B40">
         <v>2016</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B41">
         <v>2016</v>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B42">
         <v>2016</v>
@@ -2193,7 +2193,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B43">
         <v>2016</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B44">
         <v>2016</v>
@@ -2269,7 +2269,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B45">
         <v>2016</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B46">
         <v>2016</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B47">
         <v>2016</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B48">
         <v>2016</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B49">
         <v>2016</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B50">
         <v>2016</v>
@@ -2497,7 +2497,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B51">
         <v>2016</v>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B52">
         <v>2016</v>
@@ -2573,7 +2573,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B53">
         <v>2017</v>
@@ -2611,7 +2611,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B54">
         <v>2017</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B55">
         <v>2017</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B56">
         <v>2017</v>
@@ -2725,7 +2725,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B57">
         <v>2017</v>
@@ -2763,7 +2763,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B58">
         <v>2017</v>
@@ -2801,7 +2801,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B59">
         <v>2017</v>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B60">
         <v>2017</v>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B61">
         <v>2017</v>
@@ -2915,7 +2915,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B62">
         <v>2017</v>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B63">
         <v>2017</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B64">
         <v>2017</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B65">
         <v>2017</v>
@@ -3067,7 +3067,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B66">
         <v>2017</v>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B67">
         <v>2017</v>
@@ -3143,7 +3143,7 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B68">
         <v>2017</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B69">
         <v>2017</v>
@@ -3219,7 +3219,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B70">
         <v>2018</v>
@@ -3257,7 +3257,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B71">
         <v>2018</v>
@@ -3295,7 +3295,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B72">
         <v>2018</v>
@@ -3333,7 +3333,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B73">
         <v>2018</v>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B74">
         <v>2018</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B75">
         <v>2018</v>
@@ -3447,7 +3447,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B76">
         <v>2018</v>
@@ -3485,7 +3485,7 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B77">
         <v>2018</v>
@@ -3523,7 +3523,7 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B78">
         <v>2018</v>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B79">
         <v>2018</v>
@@ -3599,7 +3599,7 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B80">
         <v>2018</v>
@@ -3637,7 +3637,7 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B81">
         <v>2018</v>
@@ -3675,7 +3675,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B82">
         <v>2018</v>
@@ -3713,7 +3713,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B83">
         <v>2018</v>
@@ -3751,7 +3751,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B84">
         <v>2018</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B85">
         <v>2018</v>
@@ -3827,7 +3827,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B86">
         <v>2018</v>
@@ -3865,7 +3865,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B87">
         <v>2019</v>
@@ -3903,7 +3903,7 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B88">
         <v>2019</v>
@@ -3941,7 +3941,7 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B89">
         <v>2019</v>
@@ -3979,7 +3979,7 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B90">
         <v>2019</v>
@@ -4017,7 +4017,7 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B91">
         <v>2019</v>
@@ -4055,7 +4055,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B92">
         <v>2019</v>
@@ -4093,7 +4093,7 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B93">
         <v>2019</v>
@@ -4131,7 +4131,7 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B94">
         <v>2019</v>
@@ -4169,7 +4169,7 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B95">
         <v>2019</v>
@@ -4207,7 +4207,7 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B96">
         <v>2019</v>
@@ -4245,7 +4245,7 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B97">
         <v>2019</v>
@@ -4283,7 +4283,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B98">
         <v>2019</v>
@@ -4321,7 +4321,7 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B99">
         <v>2019</v>
@@ -4359,7 +4359,7 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B100">
         <v>2019</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B101">
         <v>2019</v>
@@ -4435,7 +4435,7 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B102">
         <v>2019</v>
@@ -4473,7 +4473,7 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B103">
         <v>2019</v>
@@ -4511,7 +4511,7 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B104">
         <v>2020</v>
@@ -4549,7 +4549,7 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B105">
         <v>2020</v>
@@ -4587,7 +4587,7 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B106">
         <v>2020</v>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B107">
         <v>2020</v>
@@ -4663,7 +4663,7 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B108">
         <v>2020</v>
@@ -4701,7 +4701,7 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B109">
         <v>2020</v>
@@ -4739,7 +4739,7 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B110">
         <v>2020</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B111">
         <v>2020</v>
@@ -4815,7 +4815,7 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B112">
         <v>2020</v>
@@ -4853,7 +4853,7 @@
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B113">
         <v>2020</v>
@@ -4891,7 +4891,7 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B114">
         <v>2020</v>
@@ -4929,7 +4929,7 @@
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B115">
         <v>2020</v>
@@ -4967,7 +4967,7 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B116">
         <v>2020</v>
@@ -5005,7 +5005,7 @@
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B117">
         <v>2020</v>
@@ -5043,7 +5043,7 @@
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B118">
         <v>2020</v>
@@ -5081,7 +5081,7 @@
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B119">
         <v>2020</v>
@@ -5119,7 +5119,7 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B120">
         <v>2020</v>

</xml_diff>